<commit_message>
dynamic auto-input fields are now posted one by one without redirect. can hence be used by following fields.
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/random_items.xlsx
+++ b/webroot/assets/example_surveys/random_items.xlsx
@@ -149,9 +149,6 @@
     <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[2,'carat']`</t>
   </si>
   <si>
-    <t>as.character(jsonlite::toJSON(readRDS(gzcon(url(paste0(item_list,"R/.val/rds"))))))</t>
-  </si>
-  <si>
     <t>q6</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[12,'carat']`</t>
+  </si>
+  <si>
+    <t>as.character(jsonlite::toJSON(readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))))</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -848,7 +848,7 @@
         <v>37</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="120">
@@ -905,7 +905,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>34</v>
@@ -922,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>34</v>
@@ -939,7 +939,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>34</v>
@@ -954,10 +954,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>34</v>
@@ -971,10 +971,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>34</v>
@@ -988,10 +988,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>34</v>
@@ -1005,10 +1005,10 @@
         <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>34</v>
@@ -1022,10 +1022,10 @@
         <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>34</v>
@@ -1039,10 +1039,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>34</v>
@@ -1056,10 +1056,10 @@
         <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
playing with random items, small bug fix in page
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/random_items.xlsx
+++ b/webroot/assets/example_surveys/random_items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="300" yWindow="760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t>cool</t>
   </si>
@@ -97,11 +97,6 @@
     <t>showif</t>
   </si>
   <si>
-    <t>##This is your personal training diary
-After completing it you will see graphs of your progress.
-You will also be able to use the graphs to infer whether there are lagged effects of drinking on your mood and your stamina.</t>
-  </si>
-  <si>
     <t>opencpu_session</t>
   </si>
   <si>
@@ -136,71 +131,134 @@
   </si>
   <si>
     <t>items_seen</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[1,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[2,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[12,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[11,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[10,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[9,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[8,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[7,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[6,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[5,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[4,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[3,'carat']`</t>
+  </si>
+  <si>
+    <t>as.character(jsonlite::toJSON(get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[,'table']))</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>q15</t>
+  </si>
+  <si>
+    <t>q16</t>
+  </si>
+  <si>
+    <t>q17</t>
+  </si>
+  <si>
+    <t>q18</t>
+  </si>
+  <si>
+    <t>q19</t>
+  </si>
+  <si>
+    <t>q20</t>
+  </si>
+  <si>
+    <t>q21</t>
+  </si>
+  <si>
+    <t>q22</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[16,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[17,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[18,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[19,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[20,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[21,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[22,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[15,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[14,'carat']`</t>
+  </si>
+  <si>
+    <t>`r get_opencpu_rds(paste0(random_items$item_list,"R/.val/rds"))[13,'carat']`</t>
+  </si>
+  <si>
+    <t>## Just testing how fast we can get David's items</t>
   </si>
   <si>
     <t>library(ggplot2)
 data(diamonds)
-diamonds[sample(nrow(diamonds),size = 175),]</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[1,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[2,'carat']`</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>q9</t>
-  </si>
-  <si>
-    <t>q10</t>
-  </si>
-  <si>
-    <t>q11</t>
-  </si>
-  <si>
-    <t>q12</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[3,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[4,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[5,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[7,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[6,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[8,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[9,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[10,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[11,'carat']`</t>
-  </si>
-  <si>
-    <t>`r readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))[12,'carat']`</t>
-  </si>
-  <si>
-    <t>as.character(jsonlite::toJSON(readRDS(gzcon(url(paste0(random_items$item_list,"R/.val/rds"))))))</t>
+diamonds[sample(nrow(diamonds),size = 180) ,]</t>
   </si>
 </sst>
 </file>
@@ -277,8 +335,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -375,7 +451,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -412,6 +488,15 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +533,15 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,7 +871,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -831,27 +925,27 @@
     </row>
     <row r="2" spans="1:10" ht="45">
       <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="120">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
@@ -859,218 +953,386 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45">
       <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="45">
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45">
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45">
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45">
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45">
       <c r="A10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45">
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45">
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45">
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45">
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45">
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="49">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45">
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45">
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45">
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45">
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45">
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45">
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45">
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45">
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45">
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>